<commit_message>
Update Process 2 Now work in Here even still dummy
</commit_message>
<xml_diff>
--- a/Process 2/Attachment Picture/bluerei75@gmail.com/Template terisi 1.xlsx
+++ b/Process 2/Attachment Picture/bluerei75@gmail.com/Template terisi 1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3e769a5e10715d52/Documents/UiPath/Process 2/Attachment Picture/bluerei75@gmail.com/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{9EA13C5E-5FA5-43C8-9926-1FF5E21319DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1606C0BA-2F01-4B1B-A6F3-768A332F72F9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4DB56E-25BB-43B1-8DF8-C367074779C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{014723A1-0C3B-4A9E-B770-D624A0815444}"/>
   </bookViews>
@@ -67,10 +67,10 @@
     <t>Steven Tjayadi</t>
   </si>
   <si>
-    <t>stjayadi@gmail.com</t>
-  </si>
-  <si>
     <t>YES</t>
+  </si>
+  <si>
+    <t>bluerei75@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -601,7 +601,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -630,18 +630,18 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>31734508</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>35353534</v>
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -649,7 +649,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -673,7 +673,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -714,7 +714,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="8"/>
     </row>

</xml_diff>